<commit_message>
build person register tei
</commit_message>
<xml_diff>
--- a/data/xlsx/Baernreither_Personenregister_2023.xlsx
+++ b/data/xlsx/Baernreither_Personenregister_2023.xlsx
@@ -1,24 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\hoermann\GitHub\dev-baernreither-app\data\xlsx\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -1480,9 +1472,6 @@
     <t>LudwigstorffAnton</t>
   </si>
   <si>
-    <t>LöckerJulius</t>
-  </si>
-  <si>
     <t>LobkowitzFerdinand</t>
   </si>
   <si>
@@ -1667,9 +1656,6 @@
   </si>
   <si>
     <t>ZichyAladar</t>
-  </si>
-  <si>
-    <t>FuerstenbergMax Egon</t>
   </si>
   <si>
     <t>GoluchowskiAgenor</t>
@@ -2438,11 +2424,17 @@
   <si>
     <t>KaljajewIwan</t>
   </si>
+  <si>
+    <t>FuerstenbergMaxEgon</t>
+  </si>
+  <si>
+    <t>LoeckerJulius</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2727,7 +2719,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
@@ -3310,7 +3302,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3320,8 +3312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="H96" sqref="H96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3448,7 +3440,7 @@
         <v>299</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3471,10 +3463,10 @@
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3505,13 +3497,13 @@
     </row>
     <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="D8" s="2">
         <v>1813</v>
@@ -3520,24 +3512,24 @@
         <v>1893</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="G8" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="D9" s="2">
         <v>1847</v>
@@ -3546,24 +3538,24 @@
         <v>1917</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="G9" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D10" s="2">
         <v>1846</v>
@@ -3572,22 +3564,22 @@
         <v>1909</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="G10" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D11" s="5">
         <v>1845</v>
@@ -3596,24 +3588,24 @@
         <v>1925</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="D12" s="7">
         <v>1843</v>
@@ -3622,22 +3614,22 @@
         <v>1911</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="D13" s="7">
         <v>1823</v>
@@ -3646,21 +3638,21 @@
         <v>1906</v>
       </c>
       <c r="F13" s="7" t="s">
+        <v>614</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>615</v>
+      </c>
+      <c r="H13" s="7" t="s">
         <v>616</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>617</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>145</v>
@@ -3672,24 +3664,24 @@
         <v>1911</v>
       </c>
       <c r="F14" s="29" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="D15" s="2">
         <v>1854</v>
@@ -3698,18 +3690,18 @@
         <v>1943</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="G15" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -3717,12 +3709,12 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="H16" s="2" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>22</v>
@@ -3737,18 +3729,18 @@
         <v>1898</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="G17" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>1</v>
@@ -3763,22 +3755,22 @@
         <v>1914</v>
       </c>
       <c r="F18" s="37" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D19" s="2">
         <v>1808</v>
@@ -3787,24 +3779,24 @@
         <v>1873</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="D20" s="2">
         <v>1798</v>
@@ -3813,13 +3805,13 @@
         <v>1860</v>
       </c>
       <c r="F20" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>640</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>642</v>
-      </c>
       <c r="H20" s="2" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -3845,7 +3837,7 @@
         <v>301</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3871,7 +3863,7 @@
         <v>302</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3917,13 +3909,13 @@
         <v>1915</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="G24" t="s">
         <v>304</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3943,7 +3935,7 @@
         <v>1927</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="G25" t="s">
         <v>305</v>
@@ -3995,7 +3987,7 @@
         <v>1912</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="G27" t="s">
         <v>307</v>
@@ -4021,13 +4013,13 @@
         <v>1924</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="G28" t="s">
         <v>308</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -4047,7 +4039,7 @@
         <v>1932</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="G29" s="35" t="s">
         <v>309</v>
@@ -4073,7 +4065,7 @@
         <v>1913</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="G30" t="s">
         <v>310</v>
@@ -4099,7 +4091,7 @@
         <v>1932</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="G31" t="s">
         <v>311</v>
@@ -4110,13 +4102,13 @@
     </row>
     <row r="32" spans="1:8" s="31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="30" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B32" s="30" t="s">
         <v>12</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D32" s="30">
         <v>1852</v>
@@ -4125,10 +4117,10 @@
         <v>1911</v>
       </c>
       <c r="F32" s="30" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="H32" s="30" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -4148,7 +4140,7 @@
         <v>1917</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="G33" t="s">
         <v>312</v>
@@ -4178,7 +4170,7 @@
         <v>313</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4198,7 +4190,7 @@
         <v>1904</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="G35" t="s">
         <v>314</v>
@@ -4224,7 +4216,7 @@
         <v>1924</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="G36" t="s">
         <v>315</v>
@@ -4261,23 +4253,23 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2">
         <v>1907</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -4297,7 +4289,7 @@
         <v>1909</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="G39" t="s">
         <v>317</v>
@@ -4323,7 +4315,7 @@
         <v>1940</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="G40" t="s">
         <v>318</v>
@@ -4349,7 +4341,7 @@
         <v>1949</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="G41" t="s">
         <v>319</v>
@@ -4364,7 +4356,7 @@
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="10" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
@@ -4373,7 +4365,7 @@
       </c>
       <c r="G42" s="10"/>
       <c r="H42" s="10" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -4393,7 +4385,7 @@
         <v>1899</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="G43" t="s">
         <v>320</v>
@@ -4425,7 +4417,7 @@
         <v>321</v>
       </c>
       <c r="H44" s="12" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -4462,7 +4454,7 @@
         <v>81</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="D46" s="14">
         <v>1863</v>
@@ -4471,13 +4463,13 @@
         <v>1941</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="G46" t="s">
         <v>324</v>
       </c>
       <c r="H46" s="14" t="s">
-        <v>535</v>
+        <v>762</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -4497,7 +4489,7 @@
         <v>1918</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="G47" t="s">
         <v>325</v>
@@ -4515,7 +4507,7 @@
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="H48" s="2" t="s">
         <v>157</v>
@@ -4545,7 +4537,7 @@
     </row>
     <row r="50" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>5</v>
@@ -4560,13 +4552,13 @@
         <v>1920</v>
       </c>
       <c r="F50" s="38" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="G50" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -4586,13 +4578,13 @@
         <v>1921</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="G51" t="s">
         <v>327</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -4600,7 +4592,7 @@
         <v>90</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>40</v>
@@ -4612,7 +4604,7 @@
         <v>1923</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="G52" t="s">
         <v>328</v>
@@ -4638,7 +4630,7 @@
         <v>1935</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="G53" t="s">
         <v>329</v>
@@ -4668,16 +4660,16 @@
       </c>
       <c r="G54" s="2"/>
       <c r="H54" s="15" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="D55" s="2">
         <v>1768</v>
@@ -4686,22 +4678,22 @@
         <v>1835</v>
       </c>
       <c r="F55" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="G55" s="32" t="s">
+        <v>649</v>
+      </c>
+      <c r="H55" s="15" t="s">
         <v>650</v>
-      </c>
-      <c r="G55" s="32" t="s">
-        <v>651</v>
-      </c>
-      <c r="H55" s="15" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D56" s="2">
         <v>1930</v>
@@ -4710,21 +4702,21 @@
         <v>1916</v>
       </c>
       <c r="F56" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="G56" t="s">
         <v>495</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" s="15" t="s">
         <v>496</v>
-      </c>
-      <c r="H56" s="15" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>228</v>
@@ -4736,24 +4728,24 @@
         <v>1907</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="H57" s="15" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>605</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>607</v>
-      </c>
       <c r="C58" s="2" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="D58" s="2">
         <v>1864</v>
@@ -4762,13 +4754,13 @@
         <v>1944</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G58" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="H58" s="15" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4788,13 +4780,13 @@
         <v>1908</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="G59" t="s">
         <v>331</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -4820,7 +4812,7 @@
         <v>332</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4846,7 +4838,7 @@
         <v>333</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -4864,24 +4856,24 @@
         <v>1907</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="G62" t="s">
         <v>335</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A63" s="33" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B63" s="33" t="s">
         <v>102</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="D63" s="2">
         <v>1824</v>
@@ -4890,21 +4882,21 @@
         <v>1899</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="G63" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A64" s="33" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B64" s="33" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>228</v>
@@ -4916,13 +4908,13 @@
         <v>1941</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="G64" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -4942,13 +4934,13 @@
         <v>1918</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="G65" t="s">
         <v>336</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4972,7 +4964,7 @@
         <v>338</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -4992,13 +4984,13 @@
         <v>1859</v>
       </c>
       <c r="F67" s="12" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="G67" t="s">
         <v>339</v>
       </c>
       <c r="H67" s="12" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -5016,13 +5008,13 @@
         <v>1954</v>
       </c>
       <c r="F68" s="12" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="G68" t="s">
         <v>340</v>
       </c>
       <c r="H68" s="12" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5046,16 +5038,16 @@
         <v>341</v>
       </c>
       <c r="H69" s="14" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="40" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="B70" s="40"/>
       <c r="C70" s="40" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="D70" s="40">
         <v>1877</v>
@@ -5064,24 +5056,24 @@
         <v>1905</v>
       </c>
       <c r="F70" s="40" t="s">
+        <v>759</v>
+      </c>
+      <c r="G70" t="s">
+        <v>760</v>
+      </c>
+      <c r="H70" s="40" t="s">
         <v>761</v>
-      </c>
-      <c r="G70" t="s">
-        <v>762</v>
-      </c>
-      <c r="H70" s="40" t="s">
-        <v>763</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>220</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="D71" s="2">
         <v>1842</v>
@@ -5090,18 +5082,18 @@
         <v>1916</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="G71" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>5</v>
@@ -5116,18 +5108,18 @@
         <v>1945</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="G72" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>12</v>
@@ -5142,22 +5134,22 @@
         <v>1911</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="G73" s="2"/>
       <c r="H73" s="2" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="D74" s="2">
         <v>1847</v>
@@ -5166,22 +5158,22 @@
         <v>1923</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="G74" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="2" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="D75" s="2">
         <v>1854</v>
@@ -5190,24 +5182,24 @@
         <v>1912</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="G75" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>187</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="D76" s="2">
         <v>1850</v>
@@ -5216,24 +5208,24 @@
         <v>1919</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D77" s="2">
         <v>1852</v>
@@ -5242,21 +5234,21 @@
         <v>1910</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="G77" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>157</v>
@@ -5268,13 +5260,13 @@
         <v>1914</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="G78" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5300,7 +5292,7 @@
         <v>342</v>
       </c>
       <c r="H79" s="12" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5326,7 +5318,7 @@
         <v>343</v>
       </c>
       <c r="H80" s="12" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5350,7 +5342,7 @@
         <v>344</v>
       </c>
       <c r="H81" s="12" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -5374,7 +5366,7 @@
         <v>345</v>
       </c>
       <c r="H82" s="12" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -5394,13 +5386,13 @@
         <v>1937</v>
       </c>
       <c r="F83" s="12" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="G83" t="s">
         <v>346</v>
       </c>
       <c r="H83" s="12" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -5426,7 +5418,7 @@
         <v>348</v>
       </c>
       <c r="H84" s="12" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -5446,16 +5438,16 @@
         <v>1921</v>
       </c>
       <c r="F85" s="12" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="G85" t="s">
         <v>347</v>
       </c>
       <c r="H85" s="12" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
         <v>138</v>
       </c>
@@ -5476,7 +5468,7 @@
         <v>349</v>
       </c>
       <c r="H86" s="14" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -5502,7 +5494,7 @@
         <v>351</v>
       </c>
       <c r="H87" s="10" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5522,13 +5514,13 @@
         <v>1918</v>
       </c>
       <c r="F88" s="12" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="G88" t="s">
         <v>352</v>
       </c>
       <c r="H88" s="12" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5548,13 +5540,13 @@
         <v>1962</v>
       </c>
       <c r="F89" s="12" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="G89" t="s">
         <v>353</v>
       </c>
       <c r="H89" s="12" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5574,13 +5566,13 @@
         <v>1939</v>
       </c>
       <c r="F90" s="12" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="G90" t="s">
         <v>354</v>
       </c>
       <c r="H90" s="12" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -5600,13 +5592,13 @@
         <v>1920</v>
       </c>
       <c r="F91" s="12" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="G91" t="s">
         <v>355</v>
       </c>
       <c r="H91" s="12" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -5632,7 +5624,7 @@
         <v>356</v>
       </c>
       <c r="H92" s="12" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -5658,7 +5650,7 @@
         <v>357</v>
       </c>
       <c r="H93" s="12" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5678,13 +5670,13 @@
         <v>1908</v>
       </c>
       <c r="F94" s="12" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="G94" t="s">
         <v>358</v>
       </c>
       <c r="H94" s="12" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -5704,13 +5696,13 @@
         <v>1926</v>
       </c>
       <c r="F95" s="12" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G95" t="s">
         <v>359</v>
       </c>
       <c r="H95" s="12" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5730,13 +5722,13 @@
         <v>1945</v>
       </c>
       <c r="F96" s="12" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="G96" t="s">
         <v>360</v>
       </c>
       <c r="H96" s="12" t="s">
-        <v>472</v>
+        <v>763</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -5756,7 +5748,7 @@
         <v>1929</v>
       </c>
       <c r="F97" s="12" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="G97" t="s">
         <v>361</v>
@@ -5782,7 +5774,7 @@
         <v>1910</v>
       </c>
       <c r="F98" s="14" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="G98" t="s">
         <v>362</v>
@@ -5808,7 +5800,7 @@
         <v>1916</v>
       </c>
       <c r="F99" s="12" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="G99" t="s">
         <v>363</v>
@@ -5838,12 +5830,12 @@
         <v>364</v>
       </c>
       <c r="H100" s="12" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="13" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="B101" s="14" t="s">
         <v>119</v>
@@ -5878,7 +5870,7 @@
         <v>1931</v>
       </c>
       <c r="F102" s="14" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="G102" t="s">
         <v>365</v>
@@ -5904,13 +5896,13 @@
         <v>1914</v>
       </c>
       <c r="F103" s="12" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="G103" t="s">
         <v>366</v>
       </c>
       <c r="H103" s="12" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -5950,7 +5942,7 @@
         <v>367</v>
       </c>
       <c r="H105" s="17" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -5970,7 +5962,7 @@
         <v>1910</v>
       </c>
       <c r="F106" s="12" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="G106" t="s">
         <v>368</v>
@@ -5994,7 +5986,7 @@
         <v>1918</v>
       </c>
       <c r="F107" s="12" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="G107" t="s">
         <v>369</v>
@@ -6018,7 +6010,7 @@
         <v>1908</v>
       </c>
       <c r="F108" s="12" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="G108" t="s">
         <v>370</v>
@@ -6082,7 +6074,7 @@
         <v>1917</v>
       </c>
       <c r="F111" s="12" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="G111" t="s">
         <v>371</v>
@@ -6122,7 +6114,7 @@
         <v>1927</v>
       </c>
       <c r="F113" s="12" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="G113" t="s">
         <v>372</v>
@@ -6146,13 +6138,13 @@
         <v>1932</v>
       </c>
       <c r="F114" s="14" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="G114" t="s">
         <v>373</v>
       </c>
       <c r="H114" s="14" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="115" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -6160,7 +6152,7 @@
         <v>193</v>
       </c>
       <c r="B115" s="12" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="C115" s="12" t="s">
         <v>194</v>
@@ -6172,13 +6164,13 @@
         <v>1914</v>
       </c>
       <c r="F115" s="12" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="G115" t="s">
         <v>374</v>
       </c>
       <c r="H115" s="12" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -6204,7 +6196,7 @@
         <v>375</v>
       </c>
       <c r="H116" s="12" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="117" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -6230,7 +6222,7 @@
         <v>376</v>
       </c>
       <c r="H117" s="12" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -6250,7 +6242,7 @@
         <v>1914</v>
       </c>
       <c r="F118" s="12" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="G118" t="s">
         <v>377</v>
@@ -6276,7 +6268,7 @@
         <v>1933</v>
       </c>
       <c r="F119" s="14" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="G119" t="s">
         <v>378</v>
@@ -6308,7 +6300,7 @@
         <v>379</v>
       </c>
       <c r="H120" s="12" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="121" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -6328,7 +6320,7 @@
         <v>1951</v>
       </c>
       <c r="F121" s="12" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="G121" s="12"/>
       <c r="H121" s="12" t="s">
@@ -6378,13 +6370,13 @@
         <v>1907</v>
       </c>
       <c r="F123" s="12" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="G123" t="s">
         <v>381</v>
       </c>
       <c r="H123" s="12" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -6404,13 +6396,13 @@
         <v>1921</v>
       </c>
       <c r="F124" s="12" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="G124" t="s">
         <v>382</v>
       </c>
       <c r="H124" s="12" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -6430,7 +6422,7 @@
         <v>1926</v>
       </c>
       <c r="F125" s="12" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="G125" t="s">
         <v>383</v>
@@ -6456,7 +6448,7 @@
         <v>1913</v>
       </c>
       <c r="F126" s="12" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="G126" t="s">
         <v>384</v>
@@ -6482,7 +6474,7 @@
         <v>1914</v>
       </c>
       <c r="F127" s="12" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="G127" t="s">
         <v>385</v>
@@ -6508,7 +6500,7 @@
         <v>1934</v>
       </c>
       <c r="F128" s="12" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="G128" t="s">
         <v>386</v>
@@ -6534,7 +6526,7 @@
         <v>1936</v>
       </c>
       <c r="F129" s="12" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="G129" t="s">
         <v>387</v>
@@ -6584,7 +6576,7 @@
         <v>1917</v>
       </c>
       <c r="F131" s="12" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="G131" t="s">
         <v>389</v>
@@ -6614,7 +6606,7 @@
         <v>390</v>
       </c>
       <c r="H132" s="12" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="133" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -6632,7 +6624,7 @@
         <v>1943</v>
       </c>
       <c r="F133" s="12" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="G133" t="s">
         <v>392</v>
@@ -6658,7 +6650,7 @@
         <v>1907</v>
       </c>
       <c r="F134" s="12" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="G134" t="s">
         <v>394</v>
@@ -6669,7 +6661,7 @@
     </row>
     <row r="135" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A135" s="11" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B135" s="12" t="s">
         <v>262</v>
@@ -6684,13 +6676,13 @@
         <v>1921</v>
       </c>
       <c r="F135" s="36" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="G135" s="35" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="H135" s="12" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="136" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -6734,13 +6726,13 @@
         <v>241</v>
       </c>
       <c r="F137" s="12" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="G137" t="s">
         <v>396</v>
       </c>
       <c r="H137" s="12" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="138" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -6758,13 +6750,13 @@
         <v>1915</v>
       </c>
       <c r="F138" s="12" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="G138" t="s">
         <v>397</v>
       </c>
       <c r="H138" s="12" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="139" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -6784,7 +6776,7 @@
       </c>
       <c r="G139" s="12"/>
       <c r="H139" s="12" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="140" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -6810,7 +6802,7 @@
         <v>398</v>
       </c>
       <c r="H140" s="12" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="141" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -6830,7 +6822,7 @@
         <v>1895</v>
       </c>
       <c r="F141" s="12" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="G141" t="s">
         <v>400</v>
@@ -6856,7 +6848,7 @@
         <v>1927</v>
       </c>
       <c r="F142" s="12" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="G142" t="s">
         <v>401</v>
@@ -6882,7 +6874,7 @@
         <v>1916</v>
       </c>
       <c r="F143" s="39" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="G143" t="s">
         <v>402</v>
@@ -6908,7 +6900,7 @@
         <v>1913</v>
       </c>
       <c r="F144" s="12" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="G144" t="s">
         <v>403</v>
@@ -6940,7 +6932,7 @@
         <v>404</v>
       </c>
       <c r="H145" s="12" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="146" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -6960,7 +6952,7 @@
         <v>1926</v>
       </c>
       <c r="F146" s="12" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="G146" t="s">
         <v>405</v>
@@ -6986,7 +6978,7 @@
         <v>1921</v>
       </c>
       <c r="F147" s="14" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="G147" s="14"/>
       <c r="H147" s="14" t="s">
@@ -7010,7 +7002,7 @@
         <v>1940</v>
       </c>
       <c r="F148" s="21" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="G148" t="s">
         <v>406</v>
@@ -7064,7 +7056,7 @@
         <v>408</v>
       </c>
       <c r="H150" s="26" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="151" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -7084,7 +7076,7 @@
         <v>1945</v>
       </c>
       <c r="F151" s="25" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="G151" t="s">
         <v>409</v>
@@ -7110,13 +7102,13 @@
         <v>1925</v>
       </c>
       <c r="F152" s="22" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="G152" t="s">
         <v>412</v>
       </c>
       <c r="H152" s="23" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="153" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -7134,13 +7126,13 @@
         <v>1921</v>
       </c>
       <c r="F153" s="12" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="G153" t="s">
         <v>413</v>
       </c>
       <c r="H153" s="12" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="154" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -7160,13 +7152,13 @@
         <v>1927</v>
       </c>
       <c r="F154" s="12" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="G154" t="s">
         <v>414</v>
       </c>
       <c r="H154" s="12" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="155" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -7184,13 +7176,13 @@
         <v>1941</v>
       </c>
       <c r="F155" s="12" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="G155" t="s">
         <v>415</v>
       </c>
       <c r="H155" s="10" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="156" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -7210,13 +7202,13 @@
         <v>1934</v>
       </c>
       <c r="F156" s="12" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="G156" t="s">
         <v>416</v>
       </c>
       <c r="H156" s="12" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="157" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -7242,7 +7234,7 @@
         <v>417</v>
       </c>
       <c r="H157" s="12" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
   </sheetData>

</xml_diff>